<commit_message>
Rule Violations Summary Model Builder
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESFA\DCT\ReportService1920\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C803B129-FDF2-4E30-9540-B3E88107ADDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95F742E-0EF5-428F-AD79-6FF1BA76D440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rule Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>Learner Destination and Progression Summary</t>
   </si>
@@ -84,15 +84,6 @@
     <t>Other 16-19 Funded Learners</t>
   </si>
   <si>
-    <t>Provider:  Provider ABC</t>
-  </si>
-  <si>
-    <t>UKPRN:  12345678</t>
-  </si>
-  <si>
-    <t>ILR File:  ILR-12345678-1920-20191024-102935-01.xml</t>
-  </si>
-  <si>
     <t>Apprenticeships (from 1 May 2017) Learners</t>
   </si>
   <si>
@@ -180,7 +171,169 @@
     <t>Year</t>
   </si>
   <si>
-    <t>2019/20</t>
+    <t>&amp;=RuleViolationSummary.Errors.RuleName</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Errors.Occurrences</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Errors.Message</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Warnings.RuleName</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Warnings.Message</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Warnings.Occurrences</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.Total</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.Total</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.ApplicationVersion</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FilePreparationDate</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LarsData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.OrganisationData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LargeEmployerData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.CampusIdData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.PostcodeData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.ReportGeneratedAt</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.ProviderName</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Ukprn</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.IlrFile</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.Year</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.AdvancedLoanLearningDeliveries</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.Total</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.ValidLearnerDestinationProgressions</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.InValidLearnerDestinationProgressions</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.LearnerDestinationProgressionsWithWarnings</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.TotalNoOfErrors</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.TotalNoOfLearners</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.TotalNoOfWarnings</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.TotalNoOfLearnersWithWarnings</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.Total</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.DevolvedPostcodesData</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.Apprenticeships</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.Apprenticeships</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.Apprenticeships</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.Funded1619</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.Funded1619</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.Funded1619</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.AdultSkilledFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.AdultSkilledFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.AdultSkilledFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.CommunityLearningFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.CommunityLearningFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.CommunityLearningFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.ESFFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.ESFFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.ESFFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.OtherAdultFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.OtherAdultFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.OtherAdultFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.Other1619Funded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.Other1619Funded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.Other1619Funded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.FullyValidLearners.NonFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.InValidLearners.NonFunded</t>
+  </si>
+  <si>
+    <t>&amp;=RuleViolationSummary.LearningDeliveries.NonFunded</t>
   </si>
 </sst>
 </file>
@@ -268,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -421,12 +574,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -474,9 +642,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -504,9 +669,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -540,9 +702,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -555,9 +714,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -585,17 +741,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -941,8 +1118,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -956,29 +1133,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -986,8 +1163,8 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
-        <v>21</v>
+      <c r="A4" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1001,348 +1178,437 @@
       <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="55" t="s">
+        <v>75</v>
+      </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="15"/>
     </row>
     <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="17"/>
+      <c r="A9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>74</v>
+      </c>
       <c r="C9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="59" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="42"/>
+      <c r="D11" s="39" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="24"/>
+      <c r="A12" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="57"/>
       <c r="C12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="19"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="19"/>
+      <c r="A13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>79</v>
+      </c>
       <c r="C13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="E13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="18" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="C15" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="C16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="C17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="18" t="s">
+        <v>94</v>
+      </c>
       <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="C19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="19"/>
+      <c r="A20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="C20" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="44"/>
+      <c r="A24" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="26" t="s">
+      <c r="B28" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="25"/>
+      <c r="B30" s="18" t="s">
+        <v>93</v>
+      </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
+      <c r="A31" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+      <c r="A32" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
+      <c r="A33" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
     </row>
     <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
+      <c r="A34" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
       <c r="E34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
+      <c r="A35" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="22"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
     </row>
     <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="48"/>
+      <c r="D38" s="45"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="49"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="53"/>
+      <c r="B39" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="49"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
+      <c r="A40" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
+      <c r="A41" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="49"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="48"/>
+      <c r="G41" s="44"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
+      <c r="A42" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="49"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
+      <c r="A43" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="49"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
+      <c r="A44" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="49"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
+      <c r="A45" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="49"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="50"/>
+      <c r="A46" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="46"/>
       <c r="D46" s="14"/>
     </row>
   </sheetData>
@@ -1357,14 +1623,14 @@
   <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.06640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="35.1328125" style="9" customWidth="1"/>
     <col min="2" max="2" width="64.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="42.59765625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
@@ -1379,10 +1645,16 @@
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
@@ -2138,12 +2410,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95794B27-11F0-4C83-BB79-3FD9E0EF0296}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.06640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="64.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="34.1328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="9" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2159,9 +2433,15 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>

</xml_diff>

<commit_message>
Rule Violation Summary Report Spec Updates and Issues Resolved
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Git\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95F742E-0EF5-428F-AD79-6FF1BA76D440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF669C5-8656-433C-8562-AF1E99940769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rule Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
   <si>
     <t>Learner Destination and Progression Summary</t>
   </si>
@@ -129,9 +129,6 @@
     <t xml:space="preserve">Total Number of Learner Destination and Progressions </t>
   </si>
   <si>
-    <t>Learner Destination and Progressions with Warnings</t>
-  </si>
-  <si>
     <t>Application Version:</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.InValidLearnerDestinationProgressions</t>
-  </si>
-  <si>
-    <t>&amp;=RuleViolationSummary.LearnerDestinationProgressionSummary.LearnerDestinationProgressionsWithWarnings</t>
   </si>
   <si>
     <t>&amp;=RuleViolationSummary.TotalNoOfErrors</t>
@@ -1118,21 +1112,21 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.19921875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="50.53125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" customWidth="1"/>
-    <col min="6" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="51.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
@@ -1140,62 +1134,62 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
@@ -1203,36 +1197,36 @@
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>21</v>
       </c>
@@ -1241,127 +1235,127 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
       <c r="C21" s="14"/>
       <c r="D21" s="22"/>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>9</v>
       </c>
@@ -1371,21 +1365,21 @@
       </c>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
         <v>21</v>
       </c>
@@ -1395,103 +1389,99 @@
       </c>
       <c r="D25" s="23"/>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>72</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="18"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22"/>
     </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>21</v>
       </c>
@@ -1500,60 +1490,60 @@
       <c r="D34" s="42"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="22"/>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
     </row>
-    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="41"/>
       <c r="D37" s="41"/>
     </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" s="48"/>
       <c r="D38" s="45"/>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="49"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="49"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="49"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="53" t="s">
+      <c r="B41" s="53" t="s">
         <v>58</v>
-      </c>
-      <c r="C40" s="49"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="53" t="s">
-        <v>59</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="1"/>
@@ -1561,52 +1551,52 @@
       <c r="F41" s="10"/>
       <c r="G41" s="44"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="49"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="53" t="s">
         <v>60</v>
-      </c>
-      <c r="C42" s="49"/>
-    </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>61</v>
       </c>
       <c r="C43" s="49"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="49"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="49"/>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="46"/>
       <c r="D46" s="14"/>
@@ -1626,14 +1616,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1328125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="64.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="42.59765625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="64.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1645,756 +1635,756 @@
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
     </row>
-    <row r="66" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
     </row>
-    <row r="67" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
     </row>
-    <row r="70" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
     </row>
-    <row r="71" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
     </row>
-    <row r="72" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
     </row>
-    <row r="80" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
     </row>
-    <row r="81" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
     </row>
-    <row r="82" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
     </row>
-    <row r="83" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
     </row>
-    <row r="84" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
     </row>
-    <row r="85" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
     </row>
-    <row r="86" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
     </row>
-    <row r="87" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
     </row>
-    <row r="88" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
     </row>
-    <row r="89" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
     </row>
-    <row r="90" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
     </row>
-    <row r="91" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
     </row>
-    <row r="92" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
     </row>
-    <row r="93" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
     </row>
-    <row r="94" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
     </row>
-    <row r="95" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
       <c r="D96"/>
     </row>
-    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
       <c r="D97"/>
     </row>
-    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
       <c r="D99"/>
     </row>
-    <row r="100" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
     </row>
-    <row r="101" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="8"/>
     </row>
-    <row r="102" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
     </row>
-    <row r="103" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
     </row>
-    <row r="104" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
     </row>
-    <row r="105" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="8"/>
     </row>
-    <row r="106" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="8"/>
     </row>
-    <row r="107" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="8"/>
     </row>
-    <row r="108" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="8"/>
     </row>
-    <row r="109" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
     </row>
-    <row r="110" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="8"/>
     </row>
-    <row r="111" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="8"/>
     </row>
-    <row r="112" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="8"/>
     </row>
-    <row r="113" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="8"/>
       <c r="D113"/>
     </row>
-    <row r="114" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="8"/>
       <c r="D114"/>
     </row>
-    <row r="115" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="8"/>
       <c r="D115"/>
     </row>
-    <row r="116" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="8"/>
       <c r="D116"/>
     </row>
-    <row r="117" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="8"/>
       <c r="D117"/>
     </row>
-    <row r="118" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="8"/>
       <c r="D118"/>
     </row>
-    <row r="119" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="8"/>
       <c r="D119"/>
     </row>
-    <row r="120" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="8"/>
       <c r="D120"/>
     </row>
-    <row r="121" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="8"/>
       <c r="D121"/>
     </row>
-    <row r="122" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="8"/>
       <c r="D122"/>
     </row>
-    <row r="123" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="8"/>
       <c r="D123"/>
     </row>
-    <row r="124" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="8"/>
       <c r="D124"/>
     </row>
-    <row r="125" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="8"/>
       <c r="D125"/>
     </row>
-    <row r="126" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="8"/>
       <c r="D126"/>
     </row>
-    <row r="127" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="8"/>
       <c r="D127"/>
     </row>
-    <row r="128" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="8"/>
       <c r="D128"/>
     </row>
-    <row r="129" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="8"/>
       <c r="D129"/>
     </row>
-    <row r="130" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="8"/>
       <c r="D130"/>
     </row>
-    <row r="131" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="8"/>
       <c r="D131"/>
     </row>
-    <row r="132" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="8"/>
       <c r="D132"/>
     </row>
-    <row r="133" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
       <c r="D133"/>
     </row>
-    <row r="134" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="8"/>
       <c r="D134"/>
     </row>
-    <row r="135" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="8"/>
@@ -2414,14 +2404,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1328125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -2432,73 +2422,73 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>

</xml_diff>

<commit_message>
template changed to move the cursor to the header
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Git\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF669C5-8656-433C-8562-AF1E99940769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C747A934-6A7A-49CE-8BD3-05C8C29BC99C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rule Summary" sheetId="1" r:id="rId1"/>
@@ -1112,9 +1112,7 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
99153 Rule violation report rollover
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/RuleViolationSummaryReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-ILR-1920-ReportService\src\ESFA.DC.ILR.ReportService.Reports\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CoryWynn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C747A934-6A7A-49CE-8BD3-05C8C29BC99C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338DCA5-EBA3-4A9E-9211-C34829CDBD75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rule Summary" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Apprenticeships (from 1 May 2017) Learning Deliveries</t>
   </si>
   <si>
-    <t>Total Number of Fully Valid Learners</t>
-  </si>
-  <si>
     <t xml:space="preserve">Report generated at: </t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>&amp;=RuleViolationSummary.LearningDeliveries.NonFunded</t>
+  </si>
+  <si>
+    <t>Total Number of Valid Learners</t>
   </si>
 </sst>
 </file>
@@ -1112,19 +1112,21 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="51.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="51.1328125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="50.59765625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" style="10" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
         <v>10</v>
       </c>
@@ -1132,62 +1134,62 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="15"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="32" t="s">
         <v>3</v>
       </c>
@@ -1195,36 +1197,36 @@
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="38" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="43" t="s">
         <v>21</v>
       </c>
@@ -1233,127 +1235,127 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
       <c r="C21" s="14"/>
       <c r="D21" s="22"/>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="32" t="s">
         <v>9</v>
       </c>
@@ -1363,21 +1365,21 @@
       </c>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="43" t="s">
         <v>21</v>
       </c>
@@ -1387,99 +1389,99 @@
       </c>
       <c r="D25" s="23"/>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="18"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22"/>
     </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="28" t="s">
         <v>21</v>
       </c>
@@ -1488,60 +1490,60 @@
       <c r="D34" s="42"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="21"/>
       <c r="B36" s="22"/>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
     </row>
-    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C37" s="41"/>
       <c r="D37" s="41"/>
     </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="47" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="48"/>
       <c r="D38" s="45"/>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="49"/>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="49" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="49"/>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="49" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="1"/>
@@ -1549,52 +1551,52 @@
       <c r="F41" s="10"/>
       <c r="G41" s="44"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="49" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="49"/>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="49"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="49" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="49"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="50" t="s">
         <v>41</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="49"/>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="46"/>
       <c r="D46" s="14"/>
@@ -1614,14 +1616,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="35.1328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="64.73046875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="42.59765625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1633,756 +1635,756 @@
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
     </row>
-    <row r="66" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
     </row>
-    <row r="67" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
     </row>
-    <row r="70" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
     </row>
-    <row r="71" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
     </row>
-    <row r="72" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
     </row>
-    <row r="80" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
     </row>
-    <row r="81" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
     </row>
-    <row r="82" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
     </row>
-    <row r="83" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
     </row>
-    <row r="84" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
     </row>
-    <row r="85" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
     </row>
-    <row r="86" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
     </row>
-    <row r="87" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
     </row>
-    <row r="88" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
     </row>
-    <row r="89" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
     </row>
-    <row r="90" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
     </row>
-    <row r="91" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
     </row>
-    <row r="92" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
     </row>
-    <row r="93" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
     </row>
-    <row r="94" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
     </row>
-    <row r="95" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
       <c r="D96"/>
     </row>
-    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
       <c r="D97"/>
     </row>
-    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
       <c r="D99"/>
     </row>
-    <row r="100" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
     </row>
-    <row r="101" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="8"/>
     </row>
-    <row r="102" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
     </row>
-    <row r="103" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
     </row>
-    <row r="104" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
     </row>
-    <row r="105" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="8"/>
     </row>
-    <row r="106" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="8"/>
     </row>
-    <row r="107" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="8"/>
     </row>
-    <row r="108" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="8"/>
     </row>
-    <row r="109" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
     </row>
-    <row r="110" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="8"/>
     </row>
-    <row r="111" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="8"/>
     </row>
-    <row r="112" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.45">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="8"/>
     </row>
-    <row r="113" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="8"/>
       <c r="D113"/>
     </row>
-    <row r="114" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="8"/>
       <c r="D114"/>
     </row>
-    <row r="115" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="8"/>
       <c r="D115"/>
     </row>
-    <row r="116" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="8"/>
       <c r="D116"/>
     </row>
-    <row r="117" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="8"/>
       <c r="D117"/>
     </row>
-    <row r="118" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="8"/>
       <c r="D118"/>
     </row>
-    <row r="119" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="8"/>
       <c r="D119"/>
     </row>
-    <row r="120" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="8"/>
       <c r="D120"/>
     </row>
-    <row r="121" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="8"/>
       <c r="D121"/>
     </row>
-    <row r="122" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="8"/>
       <c r="D122"/>
     </row>
-    <row r="123" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="8"/>
       <c r="D123"/>
     </row>
-    <row r="124" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="8"/>
       <c r="D124"/>
     </row>
-    <row r="125" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="8"/>
       <c r="D125"/>
     </row>
-    <row r="126" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="8"/>
       <c r="D126"/>
     </row>
-    <row r="127" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="8"/>
       <c r="D127"/>
     </row>
-    <row r="128" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="8"/>
       <c r="D128"/>
     </row>
-    <row r="129" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="8"/>
       <c r="D129"/>
     </row>
-    <row r="130" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="8"/>
       <c r="D130"/>
     </row>
-    <row r="131" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="8"/>
       <c r="D131"/>
     </row>
-    <row r="132" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="8"/>
       <c r="D132"/>
     </row>
-    <row r="133" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
       <c r="D133"/>
     </row>
-    <row r="134" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="8"/>
       <c r="D134"/>
     </row>
-    <row r="135" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="8"/>
@@ -2402,14 +2404,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="34.1328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -2420,73 +2422,73 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>

</xml_diff>